<commit_message>
updated some transformations in data processing
</commit_message>
<xml_diff>
--- a/data_processing/transformations/templates/calibrated/uganda/model_input_variables_uganda_se_calibrated.xlsx
+++ b/data_processing/transformations/templates/calibrated/uganda/model_input_variables_uganda_se_calibrated.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="78">
   <si>
     <t>subsector</t>
   </si>
@@ -42,6 +42,174 @@
   </si>
   <si>
     <t>min_55</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>28</t>
+  </si>
+  <si>
+    <t>29</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>31</t>
+  </si>
+  <si>
+    <t>32</t>
+  </si>
+  <si>
+    <t>33</t>
+  </si>
+  <si>
+    <t>34</t>
+  </si>
+  <si>
+    <t>35</t>
+  </si>
+  <si>
+    <t>36</t>
+  </si>
+  <si>
+    <t>37</t>
+  </si>
+  <si>
+    <t>38</t>
+  </si>
+  <si>
+    <t>39</t>
+  </si>
+  <si>
+    <t>40</t>
+  </si>
+  <si>
+    <t>41</t>
+  </si>
+  <si>
+    <t>42</t>
+  </si>
+  <si>
+    <t>43</t>
+  </si>
+  <si>
+    <t>44</t>
+  </si>
+  <si>
+    <t>45</t>
+  </si>
+  <si>
+    <t>46</t>
+  </si>
+  <si>
+    <t>47</t>
+  </si>
+  <si>
+    <t>48</t>
+  </si>
+  <si>
+    <t>49</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>51</t>
+  </si>
+  <si>
+    <t>52</t>
+  </si>
+  <si>
+    <t>53</t>
+  </si>
+  <si>
+    <t>54</t>
+  </si>
+  <si>
+    <t>55</t>
   </si>
   <si>
     <t>Economy</t>
@@ -472,181 +640,181 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1">
-        <v>0</v>
-      </c>
-      <c r="K1" s="1">
-        <v>1</v>
-      </c>
-      <c r="L1" s="1">
-        <v>2</v>
-      </c>
-      <c r="M1" s="1">
-        <v>3</v>
-      </c>
-      <c r="N1" s="1">
-        <v>4</v>
-      </c>
-      <c r="O1" s="1">
-        <v>5</v>
-      </c>
-      <c r="P1" s="1">
-        <v>6</v>
-      </c>
-      <c r="Q1" s="1">
-        <v>7</v>
-      </c>
-      <c r="R1" s="1">
-        <v>8</v>
-      </c>
-      <c r="S1" s="1">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="T1" s="1">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="U1" s="1">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="V1" s="1">
+      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="W1" s="1">
+      <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="X1" s="1">
+      <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="Y1" s="1">
+      <c r="P1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Z1" s="1">
+      <c r="Q1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="AA1" s="1">
+      <c r="R1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="AB1" s="1">
+      <c r="S1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="AC1" s="1">
+      <c r="T1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="AD1" s="1">
+      <c r="U1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="AE1" s="1">
+      <c r="V1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="AF1" s="1">
+      <c r="W1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="AG1" s="1">
+      <c r="X1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="AH1" s="1">
+      <c r="Y1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="AI1" s="1">
+      <c r="Z1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AJ1" s="1">
+      <c r="AA1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AK1" s="1">
+      <c r="AB1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AL1" s="1">
+      <c r="AC1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AM1" s="1">
+      <c r="AD1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AN1" s="1">
+      <c r="AE1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AO1" s="1">
+      <c r="AF1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AP1" s="1">
+      <c r="AG1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AQ1" s="1">
+      <c r="AH1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AR1" s="1">
+      <c r="AI1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="AS1" s="1">
+      <c r="AJ1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="AT1" s="1">
+      <c r="AK1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AU1" s="1">
+      <c r="AL1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="AV1" s="1">
+      <c r="AM1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="AW1" s="1">
+      <c r="AN1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="AX1" s="1">
+      <c r="AO1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="AY1" s="1">
+      <c r="AP1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="AZ1" s="1">
+      <c r="AQ1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="BA1" s="1">
+      <c r="AR1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="BB1" s="1">
+      <c r="AS1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="BC1" s="1">
+      <c r="AT1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="BD1" s="1">
+      <c r="AU1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="BE1" s="1">
+      <c r="AV1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="BF1" s="1">
+      <c r="AW1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="BG1" s="1">
+      <c r="AX1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="BH1" s="1">
+      <c r="AY1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="BI1" s="1">
+      <c r="AZ1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="BJ1" s="1">
+      <c r="BA1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="BK1" s="1">
+      <c r="BB1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="BL1" s="1">
+      <c r="BC1" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="BM1" s="1">
+      <c r="BD1" s="1" t="s">
         <v>55</v>
+      </c>
+      <c r="BE1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="BF1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="BG1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="BH1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="BI1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="BJ1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="BK1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="BL1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="BM1" s="1" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:65">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>65</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>67</v>
       </c>
       <c r="H2">
         <v>1</v>
@@ -825,10 +993,10 @@
     </row>
     <row r="3" spans="1:65">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>66</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>68</v>
       </c>
       <c r="H3">
         <v>1</v>
@@ -1007,10 +1175,10 @@
     </row>
     <row r="4" spans="1:65">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>66</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>69</v>
       </c>
       <c r="H4">
         <v>1</v>
@@ -1189,10 +1357,10 @@
     </row>
     <row r="5" spans="1:65">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>66</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>70</v>
       </c>
       <c r="H5">
         <v>1</v>
@@ -1371,10 +1539,10 @@
     </row>
     <row r="6" spans="1:65">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>66</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>71</v>
       </c>
       <c r="H6">
         <v>1</v>
@@ -1553,10 +1721,10 @@
     </row>
     <row r="7" spans="1:65">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>66</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>72</v>
       </c>
       <c r="H7">
         <v>1</v>
@@ -1735,10 +1903,10 @@
     </row>
     <row r="8" spans="1:65">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>66</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
+        <v>73</v>
       </c>
       <c r="H8">
         <v>1</v>
@@ -1917,10 +2085,10 @@
     </row>
     <row r="9" spans="1:65">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>66</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
+        <v>74</v>
       </c>
       <c r="H9">
         <v>1</v>
@@ -2099,10 +2267,10 @@
     </row>
     <row r="10" spans="1:65">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>66</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>75</v>
       </c>
       <c r="H10">
         <v>1</v>
@@ -2281,10 +2449,10 @@
     </row>
     <row r="11" spans="1:65">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>66</v>
       </c>
       <c r="B11" t="s">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="H11">
         <v>1</v>
@@ -2463,10 +2631,10 @@
     </row>
     <row r="12" spans="1:65">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>66</v>
       </c>
       <c r="B12" t="s">
-        <v>21</v>
+        <v>77</v>
       </c>
       <c r="H12">
         <v>1</v>
@@ -2684,181 +2852,181 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1">
-        <v>0</v>
-      </c>
-      <c r="K1" s="1">
-        <v>1</v>
-      </c>
-      <c r="L1" s="1">
-        <v>2</v>
-      </c>
-      <c r="M1" s="1">
-        <v>3</v>
-      </c>
-      <c r="N1" s="1">
-        <v>4</v>
-      </c>
-      <c r="O1" s="1">
-        <v>5</v>
-      </c>
-      <c r="P1" s="1">
-        <v>6</v>
-      </c>
-      <c r="Q1" s="1">
-        <v>7</v>
-      </c>
-      <c r="R1" s="1">
-        <v>8</v>
-      </c>
-      <c r="S1" s="1">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="T1" s="1">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="U1" s="1">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="V1" s="1">
+      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="W1" s="1">
+      <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="X1" s="1">
+      <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="Y1" s="1">
+      <c r="P1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Z1" s="1">
+      <c r="Q1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="AA1" s="1">
+      <c r="R1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="AB1" s="1">
+      <c r="S1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="AC1" s="1">
+      <c r="T1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="AD1" s="1">
+      <c r="U1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="AE1" s="1">
+      <c r="V1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="AF1" s="1">
+      <c r="W1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="AG1" s="1">
+      <c r="X1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="AH1" s="1">
+      <c r="Y1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="AI1" s="1">
+      <c r="Z1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AJ1" s="1">
+      <c r="AA1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AK1" s="1">
+      <c r="AB1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AL1" s="1">
+      <c r="AC1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AM1" s="1">
+      <c r="AD1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AN1" s="1">
+      <c r="AE1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AO1" s="1">
+      <c r="AF1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AP1" s="1">
+      <c r="AG1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AQ1" s="1">
+      <c r="AH1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AR1" s="1">
+      <c r="AI1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="AS1" s="1">
+      <c r="AJ1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="AT1" s="1">
+      <c r="AK1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AU1" s="1">
+      <c r="AL1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="AV1" s="1">
+      <c r="AM1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="AW1" s="1">
+      <c r="AN1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="AX1" s="1">
+      <c r="AO1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="AY1" s="1">
+      <c r="AP1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="AZ1" s="1">
+      <c r="AQ1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="BA1" s="1">
+      <c r="AR1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="BB1" s="1">
+      <c r="AS1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="BC1" s="1">
+      <c r="AT1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="BD1" s="1">
+      <c r="AU1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="BE1" s="1">
+      <c r="AV1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="BF1" s="1">
+      <c r="AW1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="BG1" s="1">
+      <c r="AX1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="BH1" s="1">
+      <c r="AY1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="BI1" s="1">
+      <c r="AZ1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="BJ1" s="1">
+      <c r="BA1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="BK1" s="1">
+      <c r="BB1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="BL1" s="1">
+      <c r="BC1" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="BM1" s="1">
+      <c r="BD1" s="1" t="s">
         <v>55</v>
+      </c>
+      <c r="BE1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="BF1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="BG1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="BH1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="BI1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="BJ1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="BK1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="BL1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="BM1" s="1" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:65">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>66</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>71</v>
       </c>
       <c r="H2">
         <v>1</v>

</xml_diff>